<commit_message>
With duckduck company & uppercase results. comapny cache run with ngram=2. company duckduck with normalization
</commit_message>
<xml_diff>
--- a/Additional/analysis.xlsx
+++ b/Additional/analysis.xlsx
@@ -4,22 +4,22 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="8595" windowHeight="4950"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="8595" windowHeight="4950" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="duckduck general" sheetId="1" r:id="rId1"/>
+    <sheet name="duckduck company" sheetId="2" r:id="rId2"/>
+    <sheet name="Upper" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$C$546</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'duckduck company'!$A$1:$C$534</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>5,5,5</t>
   </si>
@@ -127,6 +127,48 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>False positive (company)</t>
+  </si>
+  <si>
+    <t>False negative (company)</t>
+  </si>
+  <si>
+    <t>Expected company</t>
+  </si>
+  <si>
+    <t>Confuse (company instead of other)</t>
+  </si>
+  <si>
+    <t>result company</t>
+  </si>
+  <si>
+    <t>Confuse ne (company instead of NE)</t>
+  </si>
+  <si>
+    <t>min=1 ngram=1</t>
+  </si>
+  <si>
+    <t>min=2 ngram=1</t>
+  </si>
+  <si>
+    <t>min=1 ngram=2</t>
+  </si>
+  <si>
+    <t>min=2 gram=2</t>
+  </si>
+  <si>
+    <t>Total error (FP +FN)</t>
+  </si>
+  <si>
+    <t>Name Recall</t>
+  </si>
+  <si>
+    <t>Expected names</t>
+  </si>
+  <si>
+    <t>Found names</t>
   </si>
 </sst>
 </file>
@@ -214,7 +256,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$27</c:f>
+              <c:f>'duckduck general'!$A$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -225,7 +267,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$H$1</c:f>
+              <c:f>'duckduck general'!$B$1:$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -254,7 +296,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$H$26</c:f>
+              <c:f>'duckduck general'!$B$26:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -288,7 +330,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$29</c:f>
+              <c:f>'duckduck general'!$A$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -299,7 +341,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$H$1</c:f>
+              <c:f>'duckduck general'!$B$1:$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -328,7 +370,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$28:$H$28</c:f>
+              <c:f>'duckduck general'!$B$28:$H$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -362,7 +404,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$31</c:f>
+              <c:f>'duckduck general'!$A$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -373,7 +415,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$1:$H$1</c:f>
+              <c:f>'duckduck general'!$B$1:$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -402,7 +444,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$H$30</c:f>
+              <c:f>'duckduck general'!$B$30:$H$30</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -431,24 +473,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="102980608"/>
-        <c:axId val="75411840"/>
+        <c:axId val="78871168"/>
+        <c:axId val="78889344"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="102980608"/>
+        <c:axId val="78871168"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75411840"/>
+        <c:crossAx val="78889344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75411840"/>
+        <c:axId val="78889344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -456,7 +498,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="102980608"/>
+        <c:crossAx val="78871168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -469,7 +511,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -797,8 +839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1240,31 +1282,31 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <f>$I$2-B18</f>
+        <f t="shared" ref="B17:H17" si="0">$I$2-B18</f>
         <v>851</v>
       </c>
       <c r="C17">
-        <f>$I$2-C18</f>
+        <f t="shared" si="0"/>
         <v>409</v>
       </c>
       <c r="D17">
-        <f>$I$2-D18</f>
+        <f t="shared" si="0"/>
         <v>284</v>
       </c>
       <c r="E17">
-        <f>$I$2-E18</f>
+        <f t="shared" si="0"/>
         <v>357</v>
       </c>
       <c r="F17">
-        <f>$I$2-F18</f>
+        <f t="shared" si="0"/>
         <v>531</v>
       </c>
       <c r="G17">
-        <f>$I$2-G18</f>
+        <f t="shared" si="0"/>
         <v>500</v>
       </c>
       <c r="H17">
-        <f>$I$2-H18</f>
+        <f t="shared" si="0"/>
         <v>138</v>
       </c>
     </row>
@@ -1299,31 +1341,31 @@
         <v>14</v>
       </c>
       <c r="B20" s="3">
-        <f>B9+B5+B4</f>
+        <f t="shared" ref="B20:H20" si="1">B9+B5+B4</f>
         <v>683</v>
       </c>
       <c r="C20" s="3">
-        <f>C9+C5+C4</f>
+        <f t="shared" si="1"/>
         <v>462</v>
       </c>
       <c r="D20" s="3">
-        <f>D9+D5+D4</f>
+        <f t="shared" si="1"/>
         <v>445</v>
       </c>
       <c r="E20" s="3">
-        <f>E9+E5+E4</f>
+        <f t="shared" si="1"/>
         <v>447</v>
       </c>
       <c r="F20" s="3">
-        <f>F9+F5+F4</f>
+        <f t="shared" si="1"/>
         <v>512</v>
       </c>
       <c r="G20" s="3">
-        <f>G9+G5+G4</f>
+        <f t="shared" si="1"/>
         <v>489</v>
       </c>
       <c r="H20" s="3">
-        <f>H9+H5+H4</f>
+        <f t="shared" si="1"/>
         <v>443</v>
       </c>
     </row>
@@ -1336,15 +1378,15 @@
         <v>241</v>
       </c>
       <c r="C21" s="3">
-        <f t="shared" ref="C21:D21" si="0">C6+C10+C4</f>
+        <f t="shared" ref="C21:D21" si="2">C6+C10+C4</f>
         <v>161</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>132</v>
       </c>
       <c r="E21" s="3">
-        <f t="shared" ref="E21:G21" si="1">E6+E10+E4</f>
+        <f t="shared" ref="E21:G21" si="3">E6+E10+E4</f>
         <v>143</v>
       </c>
       <c r="F21" s="3">
@@ -1352,11 +1394,11 @@
         <v>145</v>
       </c>
       <c r="G21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>164</v>
       </c>
       <c r="H21" s="3">
-        <f t="shared" ref="H21" si="2">H6+H10+H4</f>
+        <f t="shared" ref="H21" si="4">H6+H10+H4</f>
         <v>117</v>
       </c>
     </row>
@@ -1365,19 +1407,19 @@
         <v>27</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" ref="B22:D23" si="3">B7+B11+B5</f>
+        <f t="shared" ref="B22:D23" si="5">B7+B11+B5</f>
         <v>417</v>
       </c>
       <c r="C22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>440</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>523</v>
       </c>
       <c r="E22" s="3">
-        <f t="shared" ref="E22:G22" si="4">E7+E11+E5</f>
+        <f t="shared" ref="E22:G22" si="6">E7+E11+E5</f>
         <v>462</v>
       </c>
       <c r="F22" s="3">
@@ -1385,11 +1427,11 @@
         <v>384</v>
       </c>
       <c r="G22" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>441</v>
       </c>
       <c r="H22" s="3">
-        <f t="shared" ref="H22" si="5">H7+H11+H5</f>
+        <f t="shared" ref="H22" si="7">H7+H11+H5</f>
         <v>588</v>
       </c>
     </row>
@@ -1398,19 +1440,19 @@
         <v>28</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>202</v>
       </c>
       <c r="C23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>195</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>203</v>
       </c>
       <c r="E23" s="3">
-        <f t="shared" ref="E23:G23" si="6">E8+E12+E6</f>
+        <f t="shared" ref="E23:G23" si="8">E8+E12+E6</f>
         <v>215</v>
       </c>
       <c r="F23" s="3">
@@ -1418,11 +1460,11 @@
         <v>277</v>
       </c>
       <c r="G23" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>179</v>
       </c>
       <c r="H23" s="3">
-        <f t="shared" ref="H23" si="7">H8+H12+H6</f>
+        <f t="shared" ref="H23" si="9">H8+H12+H6</f>
         <v>229</v>
       </c>
     </row>
@@ -1438,15 +1480,15 @@
         <v>0.79520344920506603</v>
       </c>
       <c r="C26" s="5">
-        <f t="shared" ref="C26:D26" si="8">(C2+C3)/$I$2</f>
+        <f t="shared" ref="C26:D26" si="10">(C2+C3)/$I$2</f>
         <v>0.85475613042306653</v>
       </c>
       <c r="D26" s="5">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0.85933710590137424</v>
       </c>
       <c r="E26" s="5">
-        <f t="shared" ref="E26" si="9">(E2+E3)/$I$2</f>
+        <f t="shared" ref="E26" si="11">(E2+E3)/$I$2</f>
         <v>0.85879816760980865</v>
       </c>
       <c r="F26" s="5">
@@ -1454,11 +1496,11 @@
         <v>0.84128267313392613</v>
       </c>
       <c r="G26" s="5">
-        <f t="shared" ref="G26:H26" si="10">(G2+G3)/$I$2</f>
+        <f t="shared" ref="G26:H26" si="12">(G2+G3)/$I$2</f>
         <v>0.84748046348693074</v>
       </c>
       <c r="H26" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.85987604419293995</v>
       </c>
     </row>
@@ -1471,15 +1513,15 @@
         <v>0.79385610347615199</v>
       </c>
       <c r="C27" s="4">
-        <f t="shared" ref="C27:D27" si="11">C2/$I$2</f>
+        <f t="shared" ref="C27:D27" si="13">C2/$I$2</f>
         <v>0.85367825383993534</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.8590676367555915</v>
       </c>
       <c r="E27" s="4">
-        <f t="shared" ref="E27" si="12">E2/$I$2</f>
+        <f t="shared" ref="E27" si="14">E2/$I$2</f>
         <v>0.85825922931824306</v>
       </c>
       <c r="F27" s="4">
@@ -1487,11 +1529,11 @@
         <v>0.84074373484236053</v>
       </c>
       <c r="G27" s="4">
-        <f t="shared" ref="G27:H27" si="13">G2/$I$2</f>
+        <f t="shared" ref="G27:H27" si="15">G2/$I$2</f>
         <v>0.84640258690379955</v>
       </c>
       <c r="H27" s="4">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.85987604419293995</v>
       </c>
     </row>
@@ -1508,11 +1550,11 @@
         <v>0.53056234718826412</v>
       </c>
       <c r="D28" s="5">
-        <f t="shared" ref="D28" si="14">1-(D9+D4)/D17</f>
+        <f t="shared" ref="D28" si="16">1-(D9+D4)/D17</f>
         <v>0.59507042253521125</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" ref="E28" si="15">1-(E9+E4)/E17</f>
+        <f t="shared" ref="E28" si="17">1-(E9+E4)/E17</f>
         <v>0.56022408963585435</v>
       </c>
       <c r="F28" s="4">
@@ -1520,11 +1562,11 @@
         <v>0.46892655367231639</v>
       </c>
       <c r="G28" s="5">
-        <f t="shared" ref="G28:H28" si="16">1-(G9+G4)/G17</f>
+        <f t="shared" ref="G28:H28" si="18">1-(G9+G4)/G17</f>
         <v>0.51200000000000001</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.70289855072463769</v>
       </c>
     </row>
@@ -1537,15 +1579,15 @@
         <v>0.33254994124559345</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" ref="C29:D29" si="17">1-(C3+C4+C9+C15)/C17</f>
+        <f t="shared" ref="C29:D29" si="19">1-(C3+C4+C9+C15)/C17</f>
         <v>0.49388753056234724</v>
       </c>
       <c r="D29" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>0.56338028169014087</v>
       </c>
       <c r="E29" s="4">
-        <f t="shared" ref="E29" si="18">1-(E3+E4+E9+E15)/E17</f>
+        <f t="shared" ref="E29" si="20">1-(E3+E4+E9+E15)/E17</f>
         <v>0.5266106442577031</v>
       </c>
       <c r="F29" s="4">
@@ -1553,11 +1595,11 @@
         <v>0.42749529190207158</v>
       </c>
       <c r="G29" s="4">
-        <f t="shared" ref="G29:H29" si="19">1-(G3+G4+G9+G15)/G17</f>
+        <f t="shared" ref="G29:H29" si="21">1-(G3+G4+G9+G15)/G17</f>
         <v>0.44799999999999995</v>
       </c>
       <c r="H29" s="4">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>0.69565217391304346</v>
       </c>
     </row>
@@ -1570,15 +1612,15 @@
         <v>0.72972972972972971</v>
       </c>
       <c r="C30" s="4">
-        <f t="shared" ref="C30:D30" si="20">1-(C5/$I$4)</f>
+        <f t="shared" ref="C30:D30" si="22">1-(C5/$I$4)</f>
         <v>0.54391891891891886</v>
       </c>
       <c r="D30" s="4">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>0.44256756756756754</v>
       </c>
       <c r="E30" s="4">
-        <f t="shared" ref="E30" si="21">1-(E5/$I$4)</f>
+        <f t="shared" ref="E30" si="23">1-(E5/$I$4)</f>
         <v>0.51013513513513509</v>
       </c>
       <c r="F30" s="5">
@@ -1586,11 +1628,11 @@
         <v>0.61148648648648651</v>
       </c>
       <c r="G30" s="4">
-        <f t="shared" ref="G30:H30" si="22">1-(G5/$I$4)</f>
+        <f t="shared" ref="G30:H30" si="24">1-(G5/$I$4)</f>
         <v>0.58614864864864868</v>
       </c>
       <c r="H30" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>0.32094594594594594</v>
       </c>
     </row>
@@ -1603,15 +1645,15 @@
         <v>0.6174757281553398</v>
       </c>
       <c r="C31" s="4">
-        <f t="shared" ref="C31:D31" si="23">1-(C5+C14)/$I$6</f>
+        <f t="shared" ref="C31:D31" si="25">1-(C5+C14)/$I$6</f>
         <v>0.34757281553398056</v>
       </c>
       <c r="D31" s="4">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>0.22524271844660193</v>
       </c>
       <c r="E31" s="4">
-        <f t="shared" ref="E31" si="24">1-(E5+E14)/$I$6</f>
+        <f t="shared" ref="E31" si="26">1-(E5+E14)/$I$6</f>
         <v>0.30679611650485439</v>
       </c>
       <c r="F31" s="4">
@@ -1619,11 +1661,11 @@
         <v>0.44271844660194171</v>
       </c>
       <c r="G31" s="4">
-        <f t="shared" ref="G31:H31" si="25">1-(G5+G14)/$I$6</f>
+        <f t="shared" ref="G31:H31" si="27">1-(G5+G14)/$I$6</f>
         <v>0.42912621359223302</v>
       </c>
       <c r="H31" s="4">
-        <f t="shared" si="25"/>
+        <f t="shared" si="27"/>
         <v>7.1844660194174792E-2</v>
       </c>
     </row>
@@ -1639,29 +1681,373 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.375" customWidth="1"/>
+    <col min="3" max="4" width="14.375" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>2950</v>
+      </c>
+      <c r="C2">
+        <v>3089</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15">
+      <c r="A3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+      <c r="C3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4">
+        <v>51</v>
+      </c>
+      <c r="C4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15">
+      <c r="A5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>217</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15">
+      <c r="A6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6">
+        <v>15</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15">
+      <c r="A8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8">
+        <v>355</v>
+      </c>
+      <c r="C8">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>99</v>
+      </c>
+      <c r="C9">
+        <v>99</v>
+      </c>
+      <c r="D9">
+        <v>99</v>
+      </c>
+      <c r="E9">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>3711</v>
+      </c>
+      <c r="C10">
+        <v>3711</v>
+      </c>
+      <c r="D10">
+        <v>3711</v>
+      </c>
+      <c r="E10">
+        <v>3711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <f>B5+B4+B3</f>
+        <v>343</v>
+      </c>
+      <c r="C12" s="3">
+        <f>C5+C4+C3</f>
+        <v>143</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ref="D12:E12" si="0">D5+D4+D3</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15">
+      <c r="A13" s="1"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="15">
+      <c r="A14" s="1"/>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="15">
+      <c r="A15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="4">
+        <f>B2/B10</f>
+        <v>0.79493398005928317</v>
+      </c>
+      <c r="C15" s="4">
+        <f>C2/C10</f>
+        <v>0.83239019132309355</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" ref="D15:E15" si="1">D2/D10</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15">
+      <c r="A16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4">
+        <f>1-(B5+B3)/B8</f>
+        <v>0.17746478873239435</v>
+      </c>
+      <c r="C16" s="4">
+        <f>1-(C5+C3)/C8</f>
+        <v>0.24705882352941178</v>
+      </c>
+      <c r="D16" s="4" t="e">
+        <f t="shared" ref="D16:E16" si="2">1-(D5+D3)/D8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E16" s="4" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4">
+        <f>1-(B5+B3+B6)/B8</f>
+        <v>0.13521126760563384</v>
+      </c>
+      <c r="C17" s="4">
+        <f>1-(C5+C3+C6)/C8</f>
+        <v>0.23529411764705888</v>
+      </c>
+      <c r="D17" s="4" t="e">
+        <f t="shared" ref="D17:E17" si="3">1-(D5+D3+D6)/D8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E17" s="4" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="5">
+        <f>1-(B4/B9)</f>
+        <v>0.48484848484848486</v>
+      </c>
+      <c r="C18" s="5">
+        <f>1-(C4/C9)</f>
+        <v>0.20202020202020199</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" ref="D18:E18" si="4">1-(D4/D9)</f>
+        <v>1</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15">
+      <c r="A19" s="1"/>
+      <c r="B19" s="4"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A2:B15"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" ht="15">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>2908</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15">
+      <c r="A8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9">
+        <v>3711</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15">
+      <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:2" ht="15">
+      <c r="A13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="4">
+        <f>(B2+B3)/B9</f>
+        <v>0.92104554028563734</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4">
+        <f>1-((B5)/B11)</f>
+        <v>0.67203682393555808</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15">
+      <c r="A15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="4">
+        <f>1-(B4/B10)</f>
+        <v>0.99155405405405406</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added experiments with ngram=2 (updated duckduck cache accordingly)
</commit_message>
<xml_diff>
--- a/Additional/analysis.xlsx
+++ b/Additional/analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="8595" windowHeight="4950" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="8595" windowHeight="4950"/>
   </bookViews>
   <sheets>
     <sheet name="duckduck general" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>5,5,5</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Found names</t>
+  </si>
+  <si>
+    <t>10,15,15 ngram2</t>
+  </si>
+  <si>
+    <t>20,20,20 ngram2</t>
+  </si>
+  <si>
+    <t>10,10,10 ngram2</t>
+  </si>
+  <si>
+    <t>5,5,5 ngram=2</t>
   </si>
 </sst>
 </file>
@@ -226,13 +238,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -267,59 +280,65 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'duckduck general'!$B$1:$H$1</c:f>
+              <c:f>'duckduck general'!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5,5,5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5,5,5 ngram=2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10,10,10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>10,10,10 ngram2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>10,15,15</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>10,15,10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10,15,5</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>8,8,10</c:v>
+                  <c:v>10,15,15 ngram2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20,20,20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20,20,20 ngram2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'duckduck general'!$B$26:$H$26</c:f>
+              <c:f>'duckduck general'!$B$26:$I$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.79520344920506603</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.79116141201832391</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.85475613042306653</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.85260037725680404</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.85933710590137424</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.85879816760980865</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.84128267313392613</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.84748046348693074</c:v>
+                  <c:v>0.86149285906763673</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.85987604419293995</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.86176232821341958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -341,59 +360,65 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'duckduck general'!$B$1:$H$1</c:f>
+              <c:f>'duckduck general'!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5,5,5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5,5,5 ngram=2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10,10,10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>10,10,10 ngram2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>10,15,15</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>10,15,10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10,15,5</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>8,8,10</c:v>
+                  <c:v>10,15,15 ngram2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20,20,20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20,20,20 ngram2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'duckduck general'!$B$28:$H$28</c:f>
+              <c:f>'duckduck general'!$B$28:$I$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.38542890716803757</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.38143176733780759</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.53056234718826412</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.51702127659574471</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.59507042253521125</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.56022408963585435</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.46892655367231639</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51200000000000001</c:v>
+                  <c:v>0.58806818181818188</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.70289855072463769</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69325153374233128</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,90 +440,108 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>'duckduck general'!$B$1:$H$1</c:f>
+              <c:f>'duckduck general'!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>5,5,5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>5,5,5 ngram=2</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>10,10,10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>10,10,10 ngram2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>10,15,15</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>10,15,10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10,15,5</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>8,8,10</c:v>
+                  <c:v>10,15,15 ngram2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>20,20,20</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20,20,20 ngram2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'duckduck general'!$B$30:$H$30</c:f>
+              <c:f>'duckduck general'!$B$30:$I$30</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0.72972972972972971</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.75506756756756754</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.54391891891891886</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.58952702702702697</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.44256756756756754</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.51013513513513509</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.61148648648648651</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.58614864864864868</c:v>
+                  <c:v>0.5067567567567568</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.32094594594594594</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.34797297297297303</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="78871168"/>
-        <c:axId val="78889344"/>
+        <c:axId val="103320192"/>
+        <c:axId val="103338368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="78871168"/>
+        <c:axId val="103320192"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78889344"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr baseline="0">
+                <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="he-IL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="103338368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78889344"/>
+        <c:axId val="103338368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:axPos val="r"/>
+        <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78871168"/>
+        <c:crossAx val="103320192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -511,7 +554,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -521,16 +564,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>619126</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -837,539 +880,691 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R31" sqref="R31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="30.125" customWidth="1"/>
     <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="13.375" customWidth="1"/>
+    <col min="7" max="7" width="17.625" customWidth="1"/>
+    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15">
+    <row r="1" spans="1:14" ht="15">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>34</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="1"/>
-    </row>
-    <row r="2" spans="1:10" ht="15">
+      <c r="N1" s="1"/>
+    </row>
+    <row r="2" spans="1:14" ht="15">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
         <v>2946</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
+        <v>2931</v>
+      </c>
+      <c r="D2">
         <v>3168</v>
       </c>
-      <c r="D2">
+      <c r="E2">
+        <v>3160</v>
+      </c>
+      <c r="F2">
         <v>3188</v>
       </c>
-      <c r="E2">
-        <v>3185</v>
-      </c>
-      <c r="F2">
-        <v>3120</v>
-      </c>
       <c r="G2">
-        <v>3141</v>
+        <v>3196</v>
       </c>
       <c r="H2">
         <v>3191</v>
       </c>
       <c r="I2">
-        <f>D2+D3+D4+D5+D9+D14+D15</f>
+        <v>3198</v>
+      </c>
+      <c r="J2">
+        <v>3185</v>
+      </c>
+      <c r="K2">
+        <v>3120</v>
+      </c>
+      <c r="L2">
+        <v>3141</v>
+      </c>
+      <c r="M2">
+        <f>F2+F3+F4+F5+F9+F14+F15</f>
         <v>3711</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15">
+    <row r="3" spans="1:14" ht="15">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>4</v>
       </c>
-      <c r="D3">
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
       <c r="G3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>4</v>
+      </c>
+      <c r="M3">
         <v>3119</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15">
+    <row r="4" spans="1:14" ht="15">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
         <v>67</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
+        <v>70</v>
+      </c>
+      <c r="D4">
         <v>39</v>
       </c>
-      <c r="D4">
+      <c r="E4">
+        <v>46</v>
+      </c>
+      <c r="F4">
         <v>24</v>
       </c>
-      <c r="E4">
-        <v>35</v>
-      </c>
-      <c r="F4">
-        <v>56</v>
-      </c>
       <c r="G4">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="H4">
         <v>17</v>
       </c>
       <c r="I4">
-        <f>I2-I3</f>
+        <v>17</v>
+      </c>
+      <c r="J4">
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <v>56</v>
+      </c>
+      <c r="L4">
+        <v>42</v>
+      </c>
+      <c r="M4">
+        <f>M2-M3</f>
         <v>592</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15">
+    <row r="5" spans="1:14" ht="15">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
         <v>160</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
+        <v>145</v>
+      </c>
+      <c r="D5">
         <v>270</v>
       </c>
-      <c r="D5">
+      <c r="E5">
+        <v>243</v>
+      </c>
+      <c r="F5">
         <v>330</v>
       </c>
-      <c r="E5">
-        <v>290</v>
-      </c>
-      <c r="F5">
-        <v>230</v>
-      </c>
       <c r="G5">
-        <v>245</v>
+        <v>292</v>
       </c>
       <c r="H5">
         <v>402</v>
       </c>
       <c r="I5">
+        <v>386</v>
+      </c>
+      <c r="J5">
+        <v>290</v>
+      </c>
+      <c r="K5">
+        <v>230</v>
+      </c>
+      <c r="L5">
+        <v>245</v>
+      </c>
+      <c r="M5">
         <v>77</v>
       </c>
-      <c r="J5" t="s">
+      <c r="N5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:14" ht="15" hidden="1" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6">
         <v>44</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2"/>
+      <c r="D6">
         <v>69</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>86</v>
-      </c>
-      <c r="E6">
-        <v>86</v>
-      </c>
-      <c r="F6">
-        <v>67</v>
-      </c>
-      <c r="G6">
-        <v>56</v>
       </c>
       <c r="H6">
         <v>89</v>
       </c>
-      <c r="I6">
-        <f>I4-I5</f>
+      <c r="J6">
+        <v>86</v>
+      </c>
+      <c r="K6">
+        <v>67</v>
+      </c>
+      <c r="L6">
+        <v>56</v>
+      </c>
+      <c r="M6">
+        <f>M4-M5</f>
         <v>515</v>
       </c>
-      <c r="J6" t="s">
+      <c r="N6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:14" hidden="1">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7">
         <v>82</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2"/>
+      <c r="D7">
         <v>126</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>146</v>
-      </c>
-      <c r="E7">
-        <v>128</v>
-      </c>
-      <c r="F7">
-        <v>112</v>
-      </c>
-      <c r="G7">
-        <v>116</v>
       </c>
       <c r="H7">
         <v>180</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="J7">
+        <v>128</v>
+      </c>
+      <c r="K7">
+        <v>112</v>
+      </c>
+      <c r="L7">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" hidden="1">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8">
         <v>34</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2"/>
+      <c r="D8">
         <v>75</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>98</v>
-      </c>
-      <c r="E8">
-        <v>76</v>
-      </c>
-      <c r="F8">
-        <v>51</v>
-      </c>
-      <c r="G8">
-        <v>73</v>
       </c>
       <c r="H8">
         <v>133</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" ht="15">
+      <c r="J8">
+        <v>76</v>
+      </c>
+      <c r="K8">
+        <v>51</v>
+      </c>
+      <c r="L8">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9">
         <v>456</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="2">
+        <v>483</v>
+      </c>
+      <c r="D9">
         <v>153</v>
       </c>
-      <c r="D9">
+      <c r="E9">
+        <v>181</v>
+      </c>
+      <c r="F9">
         <v>91</v>
       </c>
-      <c r="E9">
-        <v>122</v>
-      </c>
-      <c r="F9">
-        <v>226</v>
-      </c>
       <c r="G9">
-        <v>202</v>
+        <v>117</v>
       </c>
       <c r="H9">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="I9">
+        <v>33</v>
+      </c>
+      <c r="J9">
+        <v>122</v>
+      </c>
+      <c r="K9">
+        <v>226</v>
+      </c>
+      <c r="L9">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" hidden="1">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B10">
         <v>130</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2"/>
+      <c r="D10">
         <v>53</v>
-      </c>
-      <c r="D10">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <v>22</v>
       </c>
       <c r="F10">
         <v>22</v>
       </c>
-      <c r="G10">
-        <v>66</v>
-      </c>
       <c r="H10">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="J10">
+        <v>22</v>
+      </c>
+      <c r="K10">
+        <v>22</v>
+      </c>
+      <c r="L10">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" hidden="1">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11">
         <v>175</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2"/>
+      <c r="D11">
         <v>44</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>47</v>
-      </c>
-      <c r="E11">
-        <v>44</v>
-      </c>
-      <c r="F11">
-        <v>42</v>
-      </c>
-      <c r="G11">
-        <v>80</v>
       </c>
       <c r="H11">
         <v>6</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="J11">
+        <v>44</v>
+      </c>
+      <c r="K11">
+        <v>42</v>
+      </c>
+      <c r="L11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" hidden="1">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12">
         <v>124</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2"/>
+      <c r="D12">
         <v>51</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>19</v>
-      </c>
-      <c r="E12">
-        <v>53</v>
-      </c>
-      <c r="F12">
-        <v>159</v>
-      </c>
-      <c r="G12">
-        <v>50</v>
       </c>
       <c r="H12">
         <v>7</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="J12">
+        <v>53</v>
+      </c>
+      <c r="K12">
+        <v>159</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" hidden="1">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B13">
         <v>27</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="2"/>
+      <c r="D13">
         <v>5</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
       </c>
       <c r="F13">
         <v>3</v>
       </c>
-      <c r="G13">
-        <v>6</v>
-      </c>
       <c r="H13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" ht="15">
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14">
         <v>37</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="2">
+        <v>36</v>
+      </c>
+      <c r="D14">
         <v>66</v>
       </c>
-      <c r="D14">
+      <c r="E14">
+        <v>60</v>
+      </c>
+      <c r="F14">
         <v>69</v>
       </c>
-      <c r="E14">
-        <v>67</v>
-      </c>
-      <c r="F14">
-        <v>57</v>
-      </c>
       <c r="G14">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="H14">
         <v>76</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15">
+      <c r="I14">
+        <v>76</v>
+      </c>
+      <c r="J14">
+        <v>67</v>
+      </c>
+      <c r="K14">
+        <v>57</v>
+      </c>
+      <c r="L14">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B15">
         <v>40</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
+        <v>41</v>
+      </c>
+      <c r="D15">
         <v>11</v>
       </c>
-      <c r="D15">
+      <c r="E15">
+        <v>17</v>
+      </c>
+      <c r="F15">
         <v>8</v>
       </c>
-      <c r="E15">
-        <v>10</v>
-      </c>
-      <c r="F15">
-        <v>20</v>
-      </c>
       <c r="G15">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="H15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="15">
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>10</v>
+      </c>
+      <c r="K15">
+        <v>20</v>
+      </c>
+      <c r="L15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="15">
       <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="15">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" ht="15">
       <c r="A17" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B17">
-        <f t="shared" ref="B17:H17" si="0">$I$2-B18</f>
+        <f>$M$2-B18</f>
         <v>851</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f>$M$2-C18</f>
+        <v>894</v>
+      </c>
+      <c r="D17">
+        <f>$M$2-D18</f>
         <v>409</v>
       </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
+      <c r="E17">
+        <f>$M$2-E18</f>
+        <v>470</v>
+      </c>
+      <c r="F17">
+        <f>$M$2-F18</f>
         <v>284</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
+      <c r="G17">
+        <f>$M$2-G18</f>
+        <v>352</v>
+      </c>
+      <c r="H17">
+        <f>$M$2-H18</f>
+        <v>138</v>
+      </c>
+      <c r="I17">
+        <f>$M$2-I18</f>
+        <v>163</v>
+      </c>
+      <c r="J17">
+        <f>$M$2-J18</f>
         <v>357</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="0"/>
+      <c r="K17">
+        <f>$M$2-K18</f>
         <v>531</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="0"/>
+      <c r="L17">
+        <f>$M$2-L18</f>
         <v>500</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="0"/>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15">
+    </row>
+    <row r="18" spans="1:12" ht="15">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B18">
         <v>2860</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
+        <v>2817</v>
+      </c>
+      <c r="D18">
         <v>3302</v>
       </c>
-      <c r="D18">
+      <c r="E18">
+        <v>3241</v>
+      </c>
+      <c r="F18">
         <v>3427</v>
       </c>
-      <c r="E18">
-        <v>3354</v>
-      </c>
-      <c r="F18">
-        <v>3180</v>
-      </c>
       <c r="G18">
-        <v>3211</v>
+        <v>3359</v>
       </c>
       <c r="H18">
         <v>3573</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" ht="15">
+      <c r="I18">
+        <v>3548</v>
+      </c>
+      <c r="J18">
+        <v>3354</v>
+      </c>
+      <c r="K18">
+        <v>3180</v>
+      </c>
+      <c r="L18">
+        <v>3211</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15">
       <c r="A20" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B20" s="3">
-        <f t="shared" ref="B20:H20" si="1">B9+B5+B4</f>
+        <f t="shared" ref="B20:L20" si="0">B9+B5+B4</f>
         <v>683</v>
       </c>
       <c r="C20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
+        <v>698</v>
+      </c>
+      <c r="D20" s="3">
+        <f>D9+D5+D4</f>
         <v>462</v>
       </c>
-      <c r="D20" s="3">
-        <f t="shared" si="1"/>
+      <c r="E20" s="3">
+        <f t="shared" ref="E20" si="1">E9+E5+E4</f>
+        <v>470</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="0"/>
         <v>445</v>
       </c>
-      <c r="E20" s="3">
-        <f t="shared" si="1"/>
+      <c r="G20" s="3">
+        <f t="shared" si="0"/>
+        <v>437</v>
+      </c>
+      <c r="H20" s="3">
+        <f>H9+H5+H4</f>
+        <v>443</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" ref="I20" si="2">I9+I5+I4</f>
+        <v>436</v>
+      </c>
+      <c r="J20" s="3">
+        <f t="shared" si="0"/>
         <v>447</v>
       </c>
-      <c r="F20" s="3">
-        <f t="shared" si="1"/>
+      <c r="K20" s="3">
+        <f t="shared" si="0"/>
         <v>512</v>
       </c>
-      <c r="G20" s="3">
-        <f t="shared" si="1"/>
+      <c r="L20" s="3">
+        <f t="shared" si="0"/>
         <v>489</v>
       </c>
-      <c r="H20" s="3">
-        <f t="shared" si="1"/>
-        <v>443</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15">
+    </row>
+    <row r="21" spans="1:12" ht="15" hidden="1">
       <c r="A21" s="1" t="s">
         <v>29</v>
       </c>
@@ -1377,167 +1572,212 @@
         <f>B6+B10+B4</f>
         <v>241</v>
       </c>
-      <c r="C21" s="3">
-        <f t="shared" ref="C21:D21" si="2">C6+C10+C4</f>
+      <c r="C21" s="1"/>
+      <c r="D21" s="3">
+        <f>D6+D10+D4</f>
         <v>161</v>
       </c>
-      <c r="D21" s="3">
-        <f t="shared" si="2"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3">
+        <f t="shared" ref="F21" si="3">F6+F10+F4</f>
         <v>132</v>
       </c>
-      <c r="E21" s="3">
-        <f t="shared" ref="E21:G21" si="3">E6+E10+E4</f>
-        <v>143</v>
-      </c>
-      <c r="F21" s="3">
-        <f>F6+F10+F4</f>
-        <v>145</v>
-      </c>
-      <c r="G21" s="3">
-        <f t="shared" si="3"/>
-        <v>164</v>
-      </c>
+      <c r="G21" s="3"/>
       <c r="H21" s="3">
         <f t="shared" ref="H21" si="4">H6+H10+H4</f>
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" ht="15">
+      <c r="I21" s="3"/>
+      <c r="J21" s="3">
+        <f t="shared" ref="J21:L21" si="5">J6+J10+J4</f>
+        <v>143</v>
+      </c>
+      <c r="K21" s="3">
+        <f>K6+K10+K4</f>
+        <v>145</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="5"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15" hidden="1">
       <c r="A22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B22" s="3">
-        <f t="shared" ref="B22:D23" si="5">B7+B11+B5</f>
+        <f t="shared" ref="B22:F23" si="6">B7+B11+B5</f>
         <v>417</v>
       </c>
-      <c r="C22" s="3">
-        <f t="shared" si="5"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="3">
+        <f>D7+D11+D5</f>
         <v>440</v>
       </c>
-      <c r="D22" s="3">
-        <f t="shared" si="5"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3">
+        <f t="shared" si="6"/>
         <v>523</v>
       </c>
-      <c r="E22" s="3">
-        <f t="shared" ref="E22:G22" si="6">E7+E11+E5</f>
-        <v>462</v>
-      </c>
-      <c r="F22" s="3">
-        <f>F7+F11+F5</f>
-        <v>384</v>
-      </c>
-      <c r="G22" s="3">
-        <f t="shared" si="6"/>
-        <v>441</v>
-      </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="3">
         <f t="shared" ref="H22" si="7">H7+H11+H5</f>
         <v>588</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" ht="15">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3">
+        <f t="shared" ref="J22:L22" si="8">J7+J11+J5</f>
+        <v>462</v>
+      </c>
+      <c r="K22" s="3">
+        <f>K7+K11+K5</f>
+        <v>384</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="8"/>
+        <v>441</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" hidden="1">
       <c r="A23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B23" s="3">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>202</v>
       </c>
-      <c r="C23" s="3">
-        <f t="shared" si="5"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="3">
+        <f>D8+D12+D6</f>
         <v>195</v>
       </c>
-      <c r="D23" s="3">
-        <f t="shared" si="5"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3">
+        <f t="shared" si="6"/>
         <v>203</v>
       </c>
-      <c r="E23" s="3">
-        <f t="shared" ref="E23:G23" si="8">E8+E12+E6</f>
-        <v>215</v>
-      </c>
-      <c r="F23" s="3">
-        <f>F8+F12+F6</f>
-        <v>277</v>
-      </c>
-      <c r="G23" s="3">
-        <f t="shared" si="8"/>
-        <v>179</v>
-      </c>
+      <c r="G23" s="3"/>
       <c r="H23" s="3">
         <f t="shared" ref="H23" si="9">H8+H12+H6</f>
         <v>229</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" ht="15">
+      <c r="I23" s="3"/>
+      <c r="J23" s="3">
+        <f t="shared" ref="J23:L23" si="10">J8+J12+J6</f>
+        <v>215</v>
+      </c>
+      <c r="K23" s="3">
+        <f>K8+K12+K6</f>
+        <v>277</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="10"/>
+        <v>179</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15">
       <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" ht="15">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:12" ht="15">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B26" s="4">
-        <f>(B2+B3)/$I$2</f>
+        <f>(B2+B3)/$M$2</f>
         <v>0.79520344920506603</v>
       </c>
-      <c r="C26" s="5">
-        <f t="shared" ref="C26:D26" si="10">(C2+C3)/$I$2</f>
+      <c r="C26" s="4">
+        <f>(C2+C3)/$M$2</f>
+        <v>0.79116141201832391</v>
+      </c>
+      <c r="D26" s="5">
+        <f>(D2+D3)/$M$2</f>
         <v>0.85475613042306653</v>
       </c>
-      <c r="D26" s="5">
-        <f t="shared" si="10"/>
+      <c r="E26" s="6">
+        <f>(E2+E3)/$M$2</f>
+        <v>0.85260037725680404</v>
+      </c>
+      <c r="F26" s="5">
+        <f>(F2+F3)/$M$2</f>
         <v>0.85933710590137424</v>
       </c>
-      <c r="E26" s="5">
-        <f t="shared" ref="E26" si="11">(E2+E3)/$I$2</f>
+      <c r="G26" s="6">
+        <f>(G2+G3)/$M$2</f>
+        <v>0.86149285906763673</v>
+      </c>
+      <c r="H26" s="5">
+        <f>(H2+H3)/$M$2</f>
+        <v>0.85987604419293995</v>
+      </c>
+      <c r="I26" s="6">
+        <f>(I2+I3)/$M$2</f>
+        <v>0.86176232821341958</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" ref="J26" si="11">(J2+J3)/$M$2</f>
         <v>0.85879816760980865</v>
       </c>
-      <c r="F26" s="5">
-        <f>(F2+F3)/$I$2</f>
+      <c r="K26" s="5">
+        <f>(K2+K3)/$M$2</f>
         <v>0.84128267313392613</v>
       </c>
-      <c r="G26" s="5">
-        <f t="shared" ref="G26:H26" si="12">(G2+G3)/$I$2</f>
+      <c r="L26" s="5">
+        <f>(L2+L3)/$M$2</f>
         <v>0.84748046348693074</v>
       </c>
-      <c r="H26" s="5">
-        <f t="shared" si="12"/>
-        <v>0.85987604419293995</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15">
+    </row>
+    <row r="27" spans="1:12" ht="15">
       <c r="A27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B27" s="4">
-        <f>B2/$I$2</f>
+        <f>B2/$M$2</f>
         <v>0.79385610347615199</v>
       </c>
       <c r="C27" s="4">
-        <f t="shared" ref="C27:D27" si="13">C2/$I$2</f>
+        <f>C2/$M$2</f>
+        <v>0.78981406628940987</v>
+      </c>
+      <c r="D27" s="4">
+        <f>D2/$M$2</f>
         <v>0.85367825383993534</v>
       </c>
-      <c r="D27" s="4">
-        <f t="shared" si="13"/>
+      <c r="E27" s="4">
+        <f>E2/$M$2</f>
+        <v>0.85152250067367286</v>
+      </c>
+      <c r="F27" s="4">
+        <f>F2/$M$2</f>
         <v>0.8590676367555915</v>
       </c>
-      <c r="E27" s="4">
-        <f t="shared" ref="E27" si="14">E2/$I$2</f>
+      <c r="G27" s="6">
+        <f>G2/$M$2</f>
+        <v>0.86122338992185399</v>
+      </c>
+      <c r="H27" s="4">
+        <f>H2/$M$2</f>
+        <v>0.85987604419293995</v>
+      </c>
+      <c r="I27" s="6">
+        <f>I2/$M$2</f>
+        <v>0.86176232821341958</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" ref="J27" si="12">J2/$M$2</f>
         <v>0.85825922931824306</v>
       </c>
-      <c r="F27" s="4">
-        <f>F2/$I$2</f>
+      <c r="K27" s="4">
+        <f>K2/$M$2</f>
         <v>0.84074373484236053</v>
       </c>
-      <c r="G27" s="4">
-        <f t="shared" ref="G27:H27" si="15">G2/$I$2</f>
+      <c r="L27" s="4">
+        <f>L2/$M$2</f>
         <v>0.84640258690379955</v>
       </c>
-      <c r="H27" s="4">
-        <f t="shared" si="15"/>
-        <v>0.85987604419293995</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="15">
+    </row>
+    <row r="28" spans="1:12" ht="15">
       <c r="A28" s="1" t="s">
         <v>17</v>
       </c>
@@ -1547,30 +1787,46 @@
       </c>
       <c r="C28" s="4">
         <f>1-(C9+C4)/C17</f>
+        <v>0.38143176733780759</v>
+      </c>
+      <c r="D28" s="4">
+        <f>1-(D9+D4)/D17</f>
         <v>0.53056234718826412</v>
       </c>
-      <c r="D28" s="5">
-        <f t="shared" ref="D28" si="16">1-(D9+D4)/D17</f>
+      <c r="E28" s="4">
+        <f>1-(E9+E4)/E17</f>
+        <v>0.51702127659574471</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" ref="F28:G28" si="13">1-(F9+F4)/F17</f>
         <v>0.59507042253521125</v>
       </c>
-      <c r="E28" s="5">
-        <f t="shared" ref="E28" si="17">1-(E9+E4)/E17</f>
+      <c r="G28" s="6">
+        <f t="shared" si="13"/>
+        <v>0.58806818181818188</v>
+      </c>
+      <c r="H28" s="5">
+        <f>1-(H9+H4)/H17</f>
+        <v>0.70289855072463769</v>
+      </c>
+      <c r="I28" s="6">
+        <f>1-(I9+I4)/I17</f>
+        <v>0.69325153374233128</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" ref="J28" si="14">1-(J9+J4)/J17</f>
         <v>0.56022408963585435</v>
       </c>
-      <c r="F28" s="4">
-        <f>1-(F9+F4)/F17</f>
+      <c r="K28" s="4">
+        <f>1-(K9+K4)/K17</f>
         <v>0.46892655367231639</v>
       </c>
-      <c r="G28" s="5">
-        <f t="shared" ref="G28:H28" si="18">1-(G9+G4)/G17</f>
+      <c r="L28" s="5">
+        <f t="shared" ref="L28" si="15">1-(L9+L4)/L17</f>
         <v>0.51200000000000001</v>
       </c>
-      <c r="H28" s="5">
-        <f t="shared" si="18"/>
-        <v>0.70289855072463769</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="15">
+    </row>
+    <row r="29" spans="1:12" ht="15">
       <c r="A29" s="1" t="s">
         <v>16</v>
       </c>
@@ -1579,98 +1835,147 @@
         <v>0.33254994124559345</v>
       </c>
       <c r="C29" s="4">
-        <f t="shared" ref="C29:D29" si="19">1-(C3+C4+C9+C15)/C17</f>
+        <f>1-(C3+C4+C9+C15)/C17</f>
+        <v>0.32997762863534674</v>
+      </c>
+      <c r="D29" s="4">
+        <f>1-(D3+D4+D9+D15)/D17</f>
         <v>0.49388753056234724</v>
       </c>
-      <c r="D29" s="4">
-        <f t="shared" si="19"/>
+      <c r="E29" s="4">
+        <f t="shared" ref="E29" si="16">1-(E3+E4+E9+E15)/E17</f>
+        <v>0.47234042553191491</v>
+      </c>
+      <c r="F29" s="4">
+        <f t="shared" ref="F29" si="17">1-(F3+F4+F9+F15)/F17</f>
         <v>0.56338028169014087</v>
       </c>
-      <c r="E29" s="4">
-        <f t="shared" ref="E29" si="20">1-(E3+E4+E9+E15)/E17</f>
+      <c r="G29" s="6">
+        <f t="shared" ref="G29" si="18">1-(G3+G4+G9+G15)/G17</f>
+        <v>0.55113636363636365</v>
+      </c>
+      <c r="H29" s="4">
+        <f>1-(H3+H4+H9+H15)/H17</f>
+        <v>0.69565217391304346</v>
+      </c>
+      <c r="I29" s="4">
+        <f t="shared" ref="I29" si="19">1-(I3+I4+I9+I15)/I17</f>
+        <v>0.68711656441717794</v>
+      </c>
+      <c r="J29" s="4">
+        <f t="shared" ref="J29" si="20">1-(J3+J4+J9+J15)/J17</f>
         <v>0.5266106442577031</v>
       </c>
-      <c r="F29" s="4">
-        <f>1-(F3+F4+F9+F15)/F17</f>
+      <c r="K29" s="4">
+        <f>1-(K3+K4+K9+K15)/K17</f>
         <v>0.42749529190207158</v>
       </c>
-      <c r="G29" s="4">
-        <f t="shared" ref="G29:H29" si="21">1-(G3+G4+G9+G15)/G17</f>
+      <c r="L29" s="4">
+        <f t="shared" ref="L29" si="21">1-(L3+L4+L9+L15)/L17</f>
         <v>0.44799999999999995</v>
       </c>
-      <c r="H29" s="4">
-        <f t="shared" si="21"/>
-        <v>0.69565217391304346</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15">
+    </row>
+    <row r="30" spans="1:12" ht="15">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B30" s="5">
-        <f>1-(B5/$I$4)</f>
+        <f>1-(B5/$M$4)</f>
         <v>0.72972972972972971</v>
       </c>
-      <c r="C30" s="4">
-        <f t="shared" ref="C30:D30" si="22">1-(C5/$I$4)</f>
+      <c r="C30" s="5">
+        <f>1-(C5/$M$4)</f>
+        <v>0.75506756756756754</v>
+      </c>
+      <c r="D30" s="4">
+        <f>1-(D5/$M$4)</f>
         <v>0.54391891891891886</v>
       </c>
-      <c r="D30" s="4">
-        <f t="shared" si="22"/>
+      <c r="E30" s="4">
+        <f>1-(E5/$M$4)</f>
+        <v>0.58952702702702697</v>
+      </c>
+      <c r="F30" s="4">
+        <f>1-(F5/$M$4)</f>
         <v>0.44256756756756754</v>
       </c>
-      <c r="E30" s="4">
-        <f t="shared" ref="E30" si="23">1-(E5/$I$4)</f>
+      <c r="G30" s="6">
+        <f>1-(G5/$M$4)</f>
+        <v>0.5067567567567568</v>
+      </c>
+      <c r="H30" s="4">
+        <f>1-(H5/$M$4)</f>
+        <v>0.32094594594594594</v>
+      </c>
+      <c r="I30" s="4">
+        <f>1-(I5/$M$4)</f>
+        <v>0.34797297297297303</v>
+      </c>
+      <c r="J30" s="4">
+        <f t="shared" ref="J30" si="22">1-(J5/$M$4)</f>
         <v>0.51013513513513509</v>
       </c>
-      <c r="F30" s="5">
-        <f>1-(F5/$I$4)</f>
+      <c r="K30" s="5">
+        <f>1-(K5/$M$4)</f>
         <v>0.61148648648648651</v>
       </c>
-      <c r="G30" s="4">
-        <f t="shared" ref="G30:H30" si="24">1-(G5/$I$4)</f>
+      <c r="L30" s="4">
+        <f>1-(L5/$M$4)</f>
         <v>0.58614864864864868</v>
       </c>
-      <c r="H30" s="4">
-        <f t="shared" si="24"/>
-        <v>0.32094594594594594</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="15">
+    </row>
+    <row r="31" spans="1:12" ht="15">
       <c r="A31" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B31" s="4">
-        <f>1-(B5+B14)/$I$6</f>
+        <f>1-(B5+B14)/$M$6</f>
         <v>0.6174757281553398</v>
       </c>
       <c r="C31" s="4">
-        <f t="shared" ref="C31:D31" si="25">1-(C5+C14)/$I$6</f>
+        <f>1-(C5+C14)/$M$6</f>
+        <v>0.64854368932038842</v>
+      </c>
+      <c r="D31" s="4">
+        <f>1-(D5+D14)/$M$6</f>
         <v>0.34757281553398056</v>
       </c>
-      <c r="D31" s="4">
-        <f t="shared" si="25"/>
+      <c r="E31" s="4">
+        <f>1-(E5+E14)/$M$6</f>
+        <v>0.4116504854368932</v>
+      </c>
+      <c r="F31" s="4">
+        <f>1-(F5+F14)/$M$6</f>
         <v>0.22524271844660193</v>
       </c>
-      <c r="E31" s="4">
-        <f t="shared" ref="E31" si="26">1-(E5+E14)/$I$6</f>
+      <c r="G31" s="6">
+        <f>1-(G5+G14)/$M$6</f>
         <v>0.30679611650485439</v>
       </c>
-      <c r="F31" s="4">
-        <f>1-(F5+F14)/$I$6</f>
+      <c r="H31" s="4">
+        <f>1-(H5+H14)/$M$6</f>
+        <v>7.1844660194174792E-2</v>
+      </c>
+      <c r="I31" s="4">
+        <f>1-(I5+I14)/$M$6</f>
+        <v>0.1029126213592233</v>
+      </c>
+      <c r="J31" s="4">
+        <f t="shared" ref="J31" si="23">1-(J5+J14)/$M$6</f>
+        <v>0.30679611650485439</v>
+      </c>
+      <c r="K31" s="4">
+        <f>1-(K5+K14)/$M$6</f>
         <v>0.44271844660194171</v>
       </c>
-      <c r="G31" s="4">
-        <f t="shared" ref="G31:H31" si="27">1-(G5+G14)/$I$6</f>
+      <c r="L31" s="4">
+        <f>1-(L5+L14)/$M$6</f>
         <v>0.42912621359223302</v>
       </c>
-      <c r="H31" s="4">
-        <f t="shared" si="27"/>
-        <v>7.1844660194174792E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="15">
+    </row>
+    <row r="32" spans="1:12" ht="15">
       <c r="A32" s="1"/>
+      <c r="C32" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1683,8 +1988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1719,6 +2024,12 @@
       <c r="C2">
         <v>3089</v>
       </c>
+      <c r="D2">
+        <v>2946</v>
+      </c>
+      <c r="E2">
+        <v>3085</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15">
       <c r="A3" s="1" t="s">
@@ -1730,6 +2041,12 @@
       <c r="C3">
         <v>14</v>
       </c>
+      <c r="D3">
+        <v>79</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15">
       <c r="A4" s="1" t="s">
@@ -1741,6 +2058,12 @@
       <c r="C4">
         <v>79</v>
       </c>
+      <c r="D4">
+        <v>51</v>
+      </c>
+      <c r="E4">
+        <v>79</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15">
       <c r="A5" s="1" t="s">
@@ -1752,6 +2075,12 @@
       <c r="C5">
         <v>50</v>
       </c>
+      <c r="D5">
+        <v>221</v>
+      </c>
+      <c r="E5">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15">
       <c r="A6" s="1" t="s">
@@ -1763,6 +2092,12 @@
       <c r="C6">
         <v>1</v>
       </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15">
       <c r="A8" s="1" t="s">
@@ -1774,6 +2109,12 @@
       <c r="C8">
         <v>85</v>
       </c>
+      <c r="D8">
+        <v>363</v>
+      </c>
+      <c r="E8">
+        <v>89</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15">
       <c r="A9" s="1" t="s">
@@ -1823,11 +2164,11 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" ref="D12:E12" si="0">D5+D4+D3</f>
-        <v>0</v>
+        <v>351</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15">
@@ -1852,11 +2193,11 @@
       </c>
       <c r="D15" s="4">
         <f t="shared" ref="D15:E15" si="1">D2/D10</f>
-        <v>0</v>
+        <v>0.79385610347615199</v>
       </c>
       <c r="E15" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.83131231473996225</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15">
@@ -1871,13 +2212,13 @@
         <f>1-(C5+C3)/C8</f>
         <v>0.24705882352941178</v>
       </c>
-      <c r="D16" s="4" t="e">
+      <c r="D16" s="4">
         <f t="shared" ref="D16:E16" si="2">1-(D5+D3)/D8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E16" s="4" t="e">
+        <v>0.17355371900826444</v>
+      </c>
+      <c r="E16" s="4">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.2359550561797753</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15">
@@ -1892,13 +2233,13 @@
         <f>1-(C5+C3+C6)/C8</f>
         <v>0.23529411764705888</v>
       </c>
-      <c r="D17" s="4" t="e">
+      <c r="D17" s="4">
         <f t="shared" ref="D17:E17" si="3">1-(D5+D3+D6)/D8</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E17" s="4" t="e">
+        <v>0.13223140495867769</v>
+      </c>
+      <c r="E17" s="4">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.2247191011235955</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15">
@@ -1915,11 +2256,11 @@
       </c>
       <c r="D18" s="5">
         <f t="shared" ref="D18:E18" si="4">1-(D4/D9)</f>
-        <v>1</v>
+        <v>0.48484848484848486</v>
       </c>
       <c r="E18" s="5">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0.20202020202020199</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15">
@@ -1936,8 +2277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2034,7 +2375,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="4">
-        <f>1-((B5)/B11)</f>
+        <f>1-(B5/B11)</f>
         <v>0.67203682393555808</v>
       </c>
     </row>

</xml_diff>